<commit_message>
still need to do the weights calculation properly
</commit_message>
<xml_diff>
--- a/app/mit_solve_confirmed_matches.xlsx
+++ b/app/mit_solve_confirmed_matches.xlsx
@@ -356,7 +356,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -436,6 +436,72 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Capital One</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>BioCellection</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2020-08-31 16:28:18.472784</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Heart Institute of the Caribbean</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Algramo-Catalyzing Reusable Packaging</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2020-08-31 16:29:51.732960</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>New Orleans Health Department</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>BioCellection</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>2020-08-31 16:49:09.109752</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>